<commit_message>
modified:   main.py 	modified:   static/questions.xlsx
</commit_message>
<xml_diff>
--- a/static/questions.xlsx
+++ b/static/questions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VsCodeProjects\examination-system-backend\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCodeProjects\examination-system-backend\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BEC021-2A98-436D-9F45-F21A6DAE8533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7F1E20-FF4A-4DE4-8A87-8C0349C89A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="6810" windowWidth="20910" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10650" yWindow="7440" windowWidth="30360" windowHeight="14370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="47">
   <si>
     <t>desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +58,134 @@
   <si>
     <t>color</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D选项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>black</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.png</t>
+  </si>
+  <si>
+    <t>3.png</t>
+  </si>
+  <si>
+    <t>4.png</t>
+  </si>
+  <si>
+    <t>5.png</t>
+  </si>
+  <si>
+    <t>6.png</t>
+  </si>
+  <si>
+    <t>7.png</t>
+  </si>
+  <si>
+    <t>8.png</t>
+  </si>
+  <si>
+    <t>9.png</t>
+  </si>
+  <si>
+    <t>10.png</t>
+  </si>
+  <si>
+    <t>11.png</t>
+  </si>
+  <si>
+    <t>12.png</t>
+  </si>
+  <si>
+    <t>13.png</t>
+  </si>
+  <si>
+    <t>14.png</t>
+  </si>
+  <si>
+    <t>15.png</t>
+  </si>
+  <si>
+    <t>16.png</t>
+  </si>
+  <si>
+    <t>17.png</t>
+  </si>
+  <si>
+    <t>18.png</t>
+  </si>
+  <si>
+    <t>19.png</t>
+  </si>
+  <si>
+    <t>20.png</t>
+  </si>
+  <si>
+    <t>21.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22.png</t>
+  </si>
+  <si>
+    <t>23.png</t>
+  </si>
+  <si>
+    <t>24.png</t>
+  </si>
+  <si>
+    <t>25.png</t>
+  </si>
+  <si>
+    <t>26.png</t>
+  </si>
+  <si>
+    <t>27.png</t>
+  </si>
+  <si>
+    <t>28.png</t>
+  </si>
+  <si>
+    <t>29.png</t>
+  </si>
+  <si>
+    <t>30.png</t>
   </si>
 </sst>
 </file>
@@ -381,13 +510,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -413,6 +545,466 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -420,4 +1012,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AE6B2D-F2AB-4373-88C0-EE200A8819CF}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>